<commit_message>
ajout CommandManager, grille de correction
</commit_message>
<xml_diff>
--- a/EquivalencesPatrons.xlsx
+++ b/EquivalencesPatrons.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/53c375d97ffe9e24/Bureau/codeCollab/realLab3/LOG121Lab3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="49" documentId="8_{A17D05D9-E569-48DB-8DCD-75AD0002C6C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D54D691F-1B9E-438C-AB3F-C22DCDD1BA62}"/>
+  <xr:revisionPtr revIDLastSave="51" documentId="8_{A17D05D9-E569-48DB-8DCD-75AD0002C6C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{797A7B53-3184-4A46-A2B4-B44ABEFF86AE}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="2370" windowWidth="20490" windowHeight="10920" xr2:uid="{880479C2-DB84-4701-897F-A3EAC77F67E8}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" xr2:uid="{880479C2-DB84-4701-897F-A3EAC77F67E8}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
   <si>
     <t>Nom de l'élément du patron (classe, méthode, etc.)</t>
   </si>
@@ -95,19 +95,16 @@
     <t>Singleton</t>
   </si>
   <si>
-    <t>ImageManager</t>
-  </si>
-  <si>
     <t>Invoker</t>
   </si>
   <si>
-    <t>ImageMenu</t>
-  </si>
-  <si>
     <t>ImageCommand</t>
   </si>
   <si>
     <t>getInstance()</t>
+  </si>
+  <si>
+    <t>CommandManager</t>
   </si>
 </sst>
 </file>
@@ -479,7 +476,7 @@
   <dimension ref="D6:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -557,7 +554,7 @@
         <v>11</v>
       </c>
       <c r="E14" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="4:5" x14ac:dyDescent="0.25">
@@ -570,10 +567,10 @@
     </row>
     <row r="16" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E16" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="4:5" x14ac:dyDescent="0.25">
@@ -589,15 +586,15 @@
         <v>19</v>
       </c>
       <c r="E18" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E19" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dernier diagramme + squelette modifié
</commit_message>
<xml_diff>
--- a/EquivalencesPatrons.xlsx
+++ b/EquivalencesPatrons.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/53c375d97ffe9e24/Bureau/codeCollab/realLab3/LOG121Lab3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="51" documentId="8_{A17D05D9-E569-48DB-8DCD-75AD0002C6C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{797A7B53-3184-4A46-A2B4-B44ABEFF86AE}"/>
+  <xr:revisionPtr revIDLastSave="54" documentId="8_{A17D05D9-E569-48DB-8DCD-75AD0002C6C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0C662C4C-1E8A-41D2-9195-9D97DBB06619}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" xr2:uid="{880479C2-DB84-4701-897F-A3EAC77F67E8}"/>
   </bookViews>
@@ -98,13 +98,13 @@
     <t>Invoker</t>
   </si>
   <si>
-    <t>ImageCommand</t>
-  </si>
-  <si>
     <t>getInstance()</t>
   </si>
   <si>
     <t>CommandManager</t>
+  </si>
+  <si>
+    <t>PerspectiveCommand</t>
   </si>
 </sst>
 </file>
@@ -143,7 +143,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -151,14 +151,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -476,7 +492,7 @@
   <dimension ref="D6:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="D6" sqref="D6:E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,115 +502,115 @@
   </cols>
   <sheetData>
     <row r="6" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D7" t="s">
+      <c r="D7" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D8" t="s">
+      <c r="D8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D9" t="s">
+      <c r="D9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D10" t="s">
+      <c r="D10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D11" t="s">
+      <c r="D11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="12" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D12" t="s">
+      <c r="D12" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="13" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D13" t="s">
+      <c r="D13" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="14" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D14" t="s">
+      <c r="D14" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D15" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D16" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D17" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D18" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D19" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="15" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D15" t="s">
-        <v>12</v>
-      </c>
-      <c r="E15" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D16" t="s">
-        <v>20</v>
-      </c>
-      <c r="E16" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D17" t="s">
-        <v>14</v>
-      </c>
-      <c r="E17" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D18" t="s">
-        <v>19</v>
-      </c>
-      <c r="E18" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D19" t="s">
-        <v>22</v>
-      </c>
-      <c r="E19" t="s">
-        <v>22</v>
+      <c r="E19" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
code last updates- cleanup- noms de fonctions
</commit_message>
<xml_diff>
--- a/EquivalencesPatrons.xlsx
+++ b/EquivalencesPatrons.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/53c375d97ffe9e24/Bureau/codeCollab/realLab3/LOG121Lab3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="93" documentId="8_{A17D05D9-E569-48DB-8DCD-75AD0002C6C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{419FC79C-6A69-4AAD-B73C-F13D4DD32F2C}"/>
+  <xr:revisionPtr revIDLastSave="98" documentId="8_{A17D05D9-E569-48DB-8DCD-75AD0002C6C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{38E9DC8B-9406-496E-BBC7-CF0F3C492A1B}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" xr2:uid="{880479C2-DB84-4701-897F-A3EAC77F67E8}"/>
   </bookViews>
@@ -86,9 +86,6 @@
     <t>ConcreteObserver</t>
   </si>
   <si>
-    <t>ImagePanel</t>
-  </si>
-  <si>
     <t>Singleton</t>
   </si>
   <si>
@@ -107,9 +104,6 @@
     <t>CommandManager, ImagePerspectivePanel</t>
   </si>
   <si>
-    <t>ZoomInCommand, ZoomOutCommand, TranslateUpCommand, TranlateDownCommand, TranslateLeftCommand, TranslateRightCommand, TranslateFreeCommand, LoadCommand, SerializeCommand, DeserializeCommand</t>
-  </si>
-  <si>
     <t>Perspective, ImagePerspectivePackage</t>
   </si>
   <si>
@@ -132,6 +126,12 @@
   </si>
   <si>
     <t>PerspectiveCommand, IPPCommand, ImageCommand</t>
+  </si>
+  <si>
+    <t>ZoomInCommand, ZoomOutCommand,  TranslateFreeCommand, LoadCommand, SerializeCommand, DeserializeCommand</t>
+  </si>
+  <si>
+    <t>ImagePanel, MainPanel</t>
   </si>
 </sst>
 </file>
@@ -524,8 +524,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{763BBCA2-5AF7-417F-B83A-3203252643E3}">
   <dimension ref="D6:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="C6" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -587,7 +587,7 @@
         <v>15</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="4:5" x14ac:dyDescent="0.25">
@@ -595,7 +595,7 @@
         <v>16</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="4:5" x14ac:dyDescent="0.25">
@@ -603,23 +603,23 @@
         <v>11</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="4:5" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="4:5" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D15" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D16" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="4:5" x14ac:dyDescent="0.25">
@@ -627,36 +627,36 @@
         <v>13</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D18" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D19" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D20" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D21" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>14</v>
@@ -664,26 +664,26 @@
     </row>
     <row r="22" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D22" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D23" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D24" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="4:5" x14ac:dyDescent="0.25">

</xml_diff>